<commit_message>
ADded some isntructions for the new additional-metadata mode
</commit_message>
<xml_diff>
--- a/test_data/collections-workbook.xlsx
+++ b/test_data/collections-workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pt/working/arkisto/ro-crate-excel/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5A90EE-6079-3042-9FD0-AA0DAC7D0155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFE1251-5CA6-DF4E-818D-B5BB159835D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="760" windowWidth="29160" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3720" yWindow="-28300" windowWidth="50740" windowHeight="23780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RepositoryObject" sheetId="1" r:id="rId1"/>
@@ -42,44 +42,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Going remove this, so you can pass in an item template that gets applied to everything eg {"@type": "File", "language": "English"}
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">	-Peter Sefton</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Can add more values via columns that end in _n
-	-Peter Sefton</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -102,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -125,17 +88,26 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <scheme val="minor"/>
+            <family val="2"/>
           </rPr>
-          <t>Note calculated values -- this could be dragged-down
-	-Peter Sefton</t>
+          <t xml:space="preserve">Note calculated values -- this could be dragged-down
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">	-Peter Sefton</t>
         </r>
       </text>
     </comment>
@@ -144,41 +116,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>@id</t>
   </si>
   <si>
-    <t>@type</t>
-  </si>
-  <si>
     <t>partOf</t>
   </si>
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>is@typePrimaryMaterial</t>
-  </si>
-  <si>
-    <t>linguisticGenre</t>
-  </si>
-  <si>
-    <t>linguisticGenre_1</t>
-  </si>
-  <si>
     <t>hasAnnotation</t>
   </si>
   <si>
     <t>hasDerivation</t>
   </si>
   <si>
-    <t>is@typeDerivedMaterial</t>
-  </si>
-  <si>
-    <t>is@typeAnnotation</t>
-  </si>
-  <si>
     <t>annotationType</t>
   </si>
   <si>
@@ -212,9 +166,6 @@
     <t>/object3/1.mp4</t>
   </si>
   <si>
-    <t>Sheet name</t>
-  </si>
-  <si>
     <t>RepositoryObject</t>
   </si>
   <si>
@@ -227,21 +178,6 @@
     <t>{"@type": "File"}</t>
   </si>
   <si>
-    <t>{"license" : "LICENSE.txt"}</t>
-  </si>
-  <si>
-    <t>Fields</t>
-  </si>
-  <si>
-    <t>@id, name, is@typeAnnotation, creator, speaker</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">@id, name, age, </t>
-  </si>
-  <si>
     <t>SingleItems</t>
   </si>
   <si>
@@ -254,9 +190,6 @@
     <t>http://purl.archive.org/language-data-commons/terms#</t>
   </si>
   <si>
-    <t>"ldac:Dialogue"</t>
-  </si>
-  <si>
     <t>object1/</t>
   </si>
   <si>
@@ -264,6 +197,30 @@
   </si>
   <si>
     <t>object3/</t>
+  </si>
+  <si>
+    <t>SheetName</t>
+  </si>
+  <si>
+    <t>/object3/1.csv</t>
+  </si>
+  <si>
+    <t>{"@type": "RepositoryObject", "license" : "LICENSE.txt"}</t>
+  </si>
+  <si>
+    <t>ldac:Dialogue</t>
+  </si>
+  <si>
+    <t>is@type_PrimaryMaterial</t>
+  </si>
+  <si>
+    <t>is@type_DerivedMaterial</t>
+  </si>
+  <si>
+    <t>is@type_Annotation</t>
+  </si>
+  <si>
+    <t>isTerm_linguisticGenre</t>
   </si>
 </sst>
 </file>
@@ -343,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -351,6 +308,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -572,7 +530,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -586,17 +544,17 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -618,64 +576,59 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD7"/>
+  <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="271" zoomScaleNormal="271" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="3" max="4" width="22.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="2" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:28" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -690,163 +643,146 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-    </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT(C2," Interview Video"),"/", ""), "o", "O", 1)</f>
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT(B2," Interview Video"),"/", ""), "o", "O", 1)</f>
         <v>Object1 Interview Video</v>
       </c>
-      <c r="E2" s="1" t="b">
+      <c r="D2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="1" t="str">
-        <f>SUBSTITUTE(B3,".mp4",".csv")</f>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>SUBSTITUTE(A3,".mp4",".csv")</f>
         <v>/object1/1.csv</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D6" si="0">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT(C3," Interview Video"),"/", ""), "o", "O", 1)</f>
-        <v>Object1 Interview Video</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="1" t="b">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT(B3,"TRANSCRIPT"),"/", ""), "o", "O", 1)</f>
+        <v>Object1TRANSCRIPT</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f t="shared" ref="C4" si="0">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT(B4," Interview Video"),"/", ""), "o", "O", 1)</f>
         <v>Object2 Interview Video</v>
       </c>
-      <c r="E4" s="1" t="b">
+      <c r="D4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="1" t="str">
-        <f>SUBSTITUTE(B5,".mp4",".csv")</f>
+      <c r="E4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f>SUBSTITUTE(A5,".mp4",".csv")</f>
         <v>/object2/1.csv</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f t="shared" ref="C5" si="1">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT(B5,"TRANSCRIPT"),"/", ""), "o", "O", 1)</f>
+        <v>Object2TRANSCRIPT</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f t="shared" ref="C6" si="2">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT(B6," Interview Video"),"/", ""), "o", "O", 1)</f>
         <v>Object3 Interview Video</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" s="1" t="b">
+      <c r="D6" t="b">
         <v>1</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Object3 Interview Video</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="1" t="str">
-        <f>SUBSTITUTE(B7,".mp4",".csv")</f>
-        <v>/object2/1.csv</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f>SUBSTITUTE(A7,".mp4",".csv")</f>
+        <v>/object3/1.csv</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="1" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT(C7," Interview Video"),"/", ""), "o", "O", 1)</f>
-        <v>Object3 Interview Video</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="1" t="b">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f t="shared" ref="C7" si="3">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT(B7,"TRANSCRIPT"),"/", ""), "o", "O", 1)</f>
+        <v>Object3TRANSCRIPT</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>16</v>
+      <c r="K7" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -867,7 +803,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -875,10 +811,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -894,9 +830,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="293" zoomScaleNormal="293" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -906,41 +844,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -955,13 +879,18 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="b">
         <v>1</v>
@@ -969,7 +898,7 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>14</v>

</xml_diff>

<commit_message>
One test failing but the jsonld is still correct
</commit_message>
<xml_diff>
--- a/test_data/collections-workbook.xlsx
+++ b/test_data/collections-workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pt/working/arkisto/ro-crate-excel/test_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pt/working/language-research-technology/ro-crate-excel/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFE1251-5CA6-DF4E-818D-B5BB159835D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FD80E5-8236-8C45-9638-E98C4D07FAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3720" yWindow="-28300" windowWidth="50740" windowHeight="23780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="760" windowWidth="29280" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RepositoryObject" sheetId="1" r:id="rId1"/>
@@ -211,9 +211,6 @@
     <t>ldac:Dialogue</t>
   </si>
   <si>
-    <t>is@type_PrimaryMaterial</t>
-  </si>
-  <si>
     <t>is@type_DerivedMaterial</t>
   </si>
   <si>
@@ -221,6 +218,9 @@
   </si>
   <si>
     <t>isTerm_linguisticGenre</t>
+  </si>
+  <si>
+    <t>isType_PrimaryMaterial</t>
   </si>
 </sst>
 </file>
@@ -300,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -308,7 +308,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -579,7 +578,7 @@
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="271" zoomScaleNormal="271" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -600,11 +599,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>31</v>
+      <c r="D1" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -613,10 +612,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>5</v>

</xml_diff>